<commit_message>
Module 1 and Module 2 Question Table Template Extract
</commit_message>
<xml_diff>
--- a/OperationalExcellence/Templates/module 1/Module-1-Decide.xlsx
+++ b/OperationalExcellence/Templates/module 1/Module-1-Decide.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codebase-simtuitive-core-dev\product-templates\OperationalExcellence\Templates\module 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2310BA7A-A324-443C-B866-4D3A0A37EAED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0481442-F8C0-410B-B960-7CC07EDD7C00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5CB4F19B-C9F1-4F26-B1F4-4784C1ABDEB1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{5CB4F19B-C9F1-4F26-B1F4-4784C1ABDEB1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="OEModule1DecideQuestion" sheetId="1" r:id="rId1"/>
+    <sheet name="LearnerUserDataTable" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="60">
   <si>
     <t>No</t>
   </si>
@@ -152,6 +153,72 @@
   <si>
     <t>All scheduled passport appointments had to be cancelled due to an intense weather condition. 
 Where do you see the Service Expectation of the Federal Government in such a scenario?</t>
+  </si>
+  <si>
+    <t>TableName</t>
+  </si>
+  <si>
+    <t>OEModule2DecideLearnerUserData</t>
+  </si>
+  <si>
+    <t>Attempt</t>
+  </si>
+  <si>
+    <t>UserEmail</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>ModuleName</t>
+  </si>
+  <si>
+    <t>UI-1</t>
+  </si>
+  <si>
+    <t>UI-2</t>
+  </si>
+  <si>
+    <t>UI-3</t>
+  </si>
+  <si>
+    <t>UI-4</t>
+  </si>
+  <si>
+    <t>UI-5</t>
+  </si>
+  <si>
+    <t>UI-6</t>
+  </si>
+  <si>
+    <t>UI-7</t>
+  </si>
+  <si>
+    <t>UI-8</t>
+  </si>
+  <si>
+    <t>UI-9</t>
+  </si>
+  <si>
+    <t>UI-10</t>
+  </si>
+  <si>
+    <t>UI-11</t>
+  </si>
+  <si>
+    <t>UI-12</t>
+  </si>
+  <si>
+    <t>UI-13</t>
+  </si>
+  <si>
+    <t>UI-15</t>
+  </si>
+  <si>
+    <t>UI-14</t>
+  </si>
+  <si>
+    <t>UI-16</t>
   </si>
 </sst>
 </file>
@@ -538,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E761E6-F95A-4BF3-81F7-E1827973A4E2}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,4 +1104,97 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C8ACF93-5E52-424F-9D13-E1212E1259FA}">
+  <dimension ref="A3:T4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="13" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="20" width="7.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:20" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>